<commit_message>
Add OrchActivity, Collections and FlowControl Tests
</commit_message>
<xml_diff>
--- a/OdfOxml/MyOfficeTable/Table2.xlsx
+++ b/OdfOxml/MyOfficeTable/Table2.xlsx
@@ -729,6 +729,13 @@
     <row r="274" ht="15"/>
     <row r="275" ht="15"/>
     <row r="276" ht="15"/>
+    <row r="277" ht="15"/>
+    <row r="278" ht="15"/>
+    <row r="279" ht="15"/>
+    <row r="280" ht="15"/>
+    <row r="281" ht="15"/>
+    <row r="282" ht="15"/>
+    <row r="283" ht="15"/>
   </sheetData>
   <pageMargins left="0.790000021457672" right="0.790000021457672" top="0.790000021457672" bottom="0.790000021457672" header="0.19680555164814" footer="0.19680555164814"/>
 </worksheet>

</xml_diff>